<commit_message>
Fixed concept for introductory chapter.
</commit_message>
<xml_diff>
--- a/thesis-structure.xlsx
+++ b/thesis-structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="0" windowWidth="25360" windowHeight="14520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="25360" windowHeight="14520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Chapter</t>
   </si>
@@ -146,6 +146,15 @@
   </si>
   <si>
     <t>A bio-inspired methodology of identifying influential nodes in complex networks</t>
+  </si>
+  <si>
+    <t>PP and Natural computing</t>
+  </si>
+  <si>
+    <t>PP applicatons</t>
+  </si>
+  <si>
+    <t>Introduction to PP</t>
   </si>
 </sst>
 </file>
@@ -643,12 +652,13 @@
   <dimension ref="B3:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10">
@@ -669,10 +679,10 @@
     </row>
     <row r="9" spans="2:10">
       <c r="C9" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="J9" t="s">
         <v>12</v>
@@ -763,6 +773,11 @@
     </row>
     <row r="25" spans="5:13">
       <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="5:13">
+      <c r="E26" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="27" spans="5:13">
       <c r="J27" t="s">

</xml_diff>

<commit_message>
Finished draft of introduction to physarum.
</commit_message>
<xml_diff>
--- a/thesis-structure.xlsx
+++ b/thesis-structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="25360" windowHeight="14520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="structure" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>Chapter</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Introduction to PP</t>
+  </si>
+  <si>
+    <t>motivation for the thesis</t>
   </si>
 </sst>
 </file>
@@ -211,7 +214,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -224,6 +227,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -232,12 +238,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -649,10 +658,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:M32"/>
+  <dimension ref="B3:M45"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -661,7 +670,7 @@
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:3">
       <c r="B3" t="s">
         <v>8</v>
       </c>
@@ -669,7 +678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:3">
       <c r="B4" t="s">
         <v>8</v>
       </c>
@@ -677,40 +686,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
+    <row r="9" spans="2:3">
       <c r="C9" t="s">
         <v>42</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
-      <c r="J9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10">
-      <c r="J10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10">
-      <c r="J11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10">
-      <c r="J12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10">
-      <c r="J13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10">
-      <c r="J14" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="17" spans="5:13">
@@ -774,68 +752,106 @@
     <row r="25" spans="5:13">
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="5:13">
-      <c r="E26" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="27" spans="5:13">
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
       <c r="J27" t="s">
-        <v>20</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="5:13">
       <c r="J28" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="5:13">
       <c r="J29" t="s">
-        <v>25</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>26</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="5:13">
       <c r="J30" t="s">
-        <v>27</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="5:13">
       <c r="J31" t="s">
-        <v>37</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="32" spans="5:13">
       <c r="J32" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="5:13">
+      <c r="E37" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="5:13">
+      <c r="J38" t="s">
+        <v>20</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="5:13">
+      <c r="J39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="5:13">
+      <c r="J40" t="s">
+        <v>25</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="5:13">
+      <c r="J41" t="s">
+        <v>27</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="5:13">
+      <c r="J42" t="s">
+        <v>37</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="43" spans="5:13">
+      <c r="J43" t="s">
         <v>40</v>
       </c>
-      <c r="M32" s="2" t="s">
+      <c r="M43" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="5:13">
+      <c r="E45" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M29" r:id="rId1"/>
-    <hyperlink ref="M30" r:id="rId2"/>
-    <hyperlink ref="M22" r:id="rId3"/>
-    <hyperlink ref="M21" r:id="rId4"/>
-    <hyperlink ref="M20" r:id="rId5"/>
-    <hyperlink ref="M27" r:id="rId6"/>
-    <hyperlink ref="M23" r:id="rId7"/>
-    <hyperlink ref="M31" r:id="rId8"/>
-    <hyperlink ref="M24" r:id="rId9"/>
-    <hyperlink ref="M32" r:id="rId10"/>
+    <hyperlink ref="M22" r:id="rId1"/>
+    <hyperlink ref="M21" r:id="rId2"/>
+    <hyperlink ref="M20" r:id="rId3"/>
+    <hyperlink ref="M23" r:id="rId4"/>
+    <hyperlink ref="M24" r:id="rId5"/>
+    <hyperlink ref="M40" r:id="rId6"/>
+    <hyperlink ref="M41" r:id="rId7"/>
+    <hyperlink ref="M38" r:id="rId8"/>
+    <hyperlink ref="M42" r:id="rId9"/>
+    <hyperlink ref="M43" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>